<commit_message>
human readable trait codings in trait display
</commit_message>
<xml_diff>
--- a/Trait Matrix.xlsx
+++ b/Trait Matrix.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Comments" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Trait codings" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="173">
   <si>
     <t xml:space="preserve">Trait Matrix</t>
   </si>
@@ -475,6 +476,123 @@
   </si>
   <si>
     <t xml:space="preserve">1.10mm x 0.56mm x 0.51mm(excluding spines)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trait name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valve Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small (&lt; 0.50mm x 0.25mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium (0.50mm-1.00mm x 0.25mm – 0.50mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large (&gt; 1.00mm x 0.50mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valve Calcification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valve Shape (dorsal view: anterior-posterior)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ovate or Subovate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectangular or Subrectangular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Surface Reticulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventral Margin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventral Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorsal Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posterior Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anterior Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right/Left Valve Size Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Valve Larger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equally Sized Valves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Valve Larger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Spines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carapace Pits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Carapace Pits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Opaque Patches on Valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Denticulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Alae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Caudal Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Sulcus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Eye Tubercules</t>
   </si>
 </sst>
 </file>
@@ -823,35 +941,35 @@
   </sheetPr>
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8582995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1619433198381"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="25" min="22" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.0364372469636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.080971659919"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7287449392713"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7004048582996"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5587044534413"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.165991902834"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.578947368421"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8825910931174"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3603238866397"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5465587044534"/>
+    <col collapsed="false" hidden="false" max="25" min="22" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.56275303643725"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2738,7 +2856,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>58</v>
       </c>
@@ -3278,28 +3396,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.080971659919"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9352226720648"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1619433198381"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="116.323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.080971659919"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7287449392713"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7004048582996"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5587044534413"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.165991902834"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.578947368421"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8825910931174"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3603238866397"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.56275303643725"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,4 +4231,325 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9392712550607"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.7004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.6113360323887"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7651821862348"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5263157894737"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
React (#6) - Fixes #2
* Basic data is being rendered. Need to fix whitespace in emacs.

* prefix searching with react works

* Filter by trait and prefix

* frontend filters by some traits

* human readable trait codings in trait display

* add requirements.txt since i'm not an animal

* read me
</commit_message>
<xml_diff>
--- a/Trait Matrix.xlsx
+++ b/Trait Matrix.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Comments" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Trait codings" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="173">
   <si>
     <t xml:space="preserve">Trait Matrix</t>
   </si>
@@ -475,6 +476,123 @@
   </si>
   <si>
     <t xml:space="preserve">1.10mm x 0.56mm x 0.51mm(excluding spines)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trait name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valve Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small (&lt; 0.50mm x 0.25mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium (0.50mm-1.00mm x 0.25mm – 0.50mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large (&gt; 1.00mm x 0.50mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valve Calcification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valve Shape (dorsal view: anterior-posterior)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ovate or Subovate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectangular or Subrectangular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Surface Reticulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventral Margin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventral Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorsal Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posterior Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anterior Margin Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right/Left Valve Size Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Valve Larger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equally Sized Valves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Valve Larger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Spines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carapace Pits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Carapace Pits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Opaque Patches on Valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Denticulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Alae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Caudal Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Sulcus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of Eye Tubercules</t>
   </si>
 </sst>
 </file>
@@ -823,35 +941,35 @@
   </sheetPr>
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8582995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1619433198381"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="25" min="22" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.0364372469636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.080971659919"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7287449392713"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7004048582996"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5587044534413"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.165991902834"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.578947368421"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8825910931174"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3603238866397"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5465587044534"/>
+    <col collapsed="false" hidden="false" max="25" min="22" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.56275303643725"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2738,7 +2856,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>58</v>
       </c>
@@ -3278,28 +3396,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.080971659919"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9352226720648"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1619433198381"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3036437246964"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.82995951417"/>
-    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="116.323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.080971659919"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7287449392713"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7004048582996"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5587044534413"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.165991902834"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.578947368421"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8825910931174"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.0364372469636"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3603238866397"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="15.7894736842105"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.56275303643725"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,4 +4231,325 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9392712550607"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.7004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.6113360323887"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7651821862348"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5263157894737"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sidebar, collapsed filters, database fixes
</commit_message>
<xml_diff>
--- a/Trait Matrix.xlsx
+++ b/Trait Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="169">
   <si>
     <t xml:space="preserve">Trait Matrix</t>
   </si>
@@ -431,18 +431,6 @@
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carapce Texture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dorsalmargin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posterior margin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leftoverlap</t>
   </si>
   <si>
     <t xml:space="preserve">Column5</t>
@@ -877,12 +865,12 @@
     <tableColumn id="3" name="Size"/>
     <tableColumn id="4" name="Calcification"/>
     <tableColumn id="5" name="Shape"/>
-    <tableColumn id="6" name="Carapce Texture"/>
+    <tableColumn id="6" name="Carapace Texture"/>
     <tableColumn id="7" name="Ventral margin"/>
-    <tableColumn id="8" name="Dorsalmargin"/>
-    <tableColumn id="9" name="Posterior margin"/>
+    <tableColumn id="8" name="Dorsal Margin"/>
+    <tableColumn id="9" name="Posterior Margin"/>
     <tableColumn id="10" name="Anterior Margin"/>
-    <tableColumn id="11" name="Leftoverlap"/>
+    <tableColumn id="11" name="Left overlap"/>
     <tableColumn id="12" name="Spines"/>
     <tableColumn id="13" name="Carapace pits"/>
     <tableColumn id="14" name="Opaque Areas"/>
@@ -942,34 +930,34 @@
   <dimension ref="A1:Y91"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="A2:T3 A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.0364372469636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.56275303643725"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.080971659919"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7287449392713"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7004048582996"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0364372469636"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5587044534413"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7894736842105"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.165991902834"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.578947368421"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.56275303643725"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8825910931174"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.0364372469636"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3603238866397"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5465587044534"/>
-    <col collapsed="false" hidden="false" max="25" min="22" style="0" width="15.7894736842105"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.7206477732794"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4574898785425"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.82995951417"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.8987854251012"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.0526315789474"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.8987854251012"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3400809716599"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="25" min="22" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="10.1781376518219"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3390,34 +3378,34 @@
   </sheetPr>
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8056680161943"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="116.323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.080971659919"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7287449392713"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7004048582996"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0364372469636"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.5587044534413"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7894736842105"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.165991902834"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.578947368421"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.56275303643725"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8825910931174"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.0364372469636"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3603238866397"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="15.7894736842105"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.56275303643725"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="123.878542510121"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.7206477732794"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4574898785425"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.82995951417"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.8987854251012"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.0526315789474"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.8987854251012"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3400809716599"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="10.1781376518219"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,7 +3413,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3442,22 +3430,22 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>12</v>
@@ -3487,7 +3475,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3504,22 +3492,22 @@
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>12</v>
@@ -3561,7 +3549,7 @@
         <v>25</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,13 +3705,13 @@
         <v>54</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3734,10 +3722,10 @@
         <v>54</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,16 +3952,16 @@
         <v>85</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N61" s="0" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3984,7 +3972,7 @@
         <v>85</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4240,25 +4228,25 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A2:T3 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9392712550607"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.7004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.6113360323887"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7651821862348"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0445344129555"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.582995951417"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5060728744939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="n">
         <v>0</v>
@@ -4275,16 +4263,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4292,16 +4280,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4309,13 +4297,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4323,30 +4311,30 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4354,16 +4342,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4371,16 +4359,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4388,33 +4376,33 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4422,27 +4410,27 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4450,13 +4438,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,13 +4452,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4478,13 +4466,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4492,13 +4480,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,13 +4494,13 @@
         <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4520,13 +4508,13 @@
         <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,13 +4522,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>